<commit_message>
Final Commit After Merge
</commit_message>
<xml_diff>
--- a/Project/testdata/data.xlsx
+++ b/Project/testdata/data.xlsx
@@ -4,6 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -397,6 +402,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Search Data</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Titles To Verify</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Filter Verifier</v>
+      </c>
+      <c r="D1" t="str">
+        <v>URL verifier</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Consumer Electronics</v>
+      </c>
+      <c r="D2" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Machine-Tools.html</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <v>ISO 9000</v>
+      </c>
+      <c r="D3" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Engineering-Construction-Machinery.html</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v>Diamond Member</v>
+      </c>
+      <c r="D4" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Woodworking-Machinery.html</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Plastic-Machinery.html</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Metallic-Processing-Machinery.html</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Mould.html</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Laser-Equipment.html</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Casting-Forging.html</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Agricultural-Machinery.html</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Products</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Wires</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Furniture</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -446,4 +583,274 @@
     <ignoredError numberStoredAsText="1" sqref="A1:A7"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Verify Title</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Verify label</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Register</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Español</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Sign In | Made-in-China.com</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Français</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>Deutsch</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>Русский язык</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>日本語</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>Manufacturing &amp; Processing Machinery</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Consumer Electronics</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>Industrial Equipment &amp; Components</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="str">
+        <v>Electrical &amp; Electronics</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>Construction &amp; Decoration</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="str">
+        <v>Light Industry &amp; Daily Use</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="str">
+        <v>Auto, Motorcycle Parts &amp; Accessories</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="str">
+        <v>Apparel &amp; Accessories</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="str">
+        <v>Lights &amp; Lighting</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="str">
+        <v>Sporting Goods &amp; Recreation</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B17"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>krushn34@gmail.com</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>how-to-source-products-on-made-in-china-com</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>audited-suppliers</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>private-sourcing-meetings</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>LED lights</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Furniture.html</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Furniture</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>I would like to inquire about your services. Please provide detailed information regarding pricing and availability at the earliest convenience</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Apparel-Clothing.html</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Apparel &amp; Clothing</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>tsr@gmail.com</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Auto-Parts-Accessories.html</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Auto Parts &amp; Accessories</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>john</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Bags-Cases-Luggages.html</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Bags, Cases &amp; Luggages</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>happy</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Computer-Products.html</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Computer Products</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1234567891</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Consumer-Electronics.html</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Consumer Electronics</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>Electrical-Equipments.html</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Electrical Equipment</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>Electronic-Components.html</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Electronic Components</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Gifts-Crafts-Collectibles.html</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Gifts, Crafts &amp; Collectibles</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>Motorcycles-Scooters.html</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Motorcycles &amp; Scooters</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="str">
+        <v>Sealing-Packaging-Storage-Shelving.html</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Sealing, Packaging, Storage &amp; Shelving</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>Building-Materials-Supplies.html</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Building Materials &amp; Supplies</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>